<commit_message>
Added benckmarks for 30 days removed lin heur for 30 days
</commit_message>
<xml_diff>
--- a/benchmarks/simulations-30.0-days.xlsx
+++ b/benchmarks/simulations-30.0-days.xlsx
@@ -498,13 +498,13 @@
         <v>13</v>
       </c>
       <c r="H2">
-        <v>6342368776.007891</v>
+        <v>6342375971.934543</v>
       </c>
       <c r="I2">
-        <v>10.19839163772356</v>
+        <v>34.25914524946653</v>
       </c>
       <c r="J2">
-        <v>6341912291.277191</v>
+        <v>6341012460.906618</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -530,13 +530,13 @@
         <v>14</v>
       </c>
       <c r="H3">
-        <v>6342368776.007891</v>
+        <v>6342375971.934543</v>
       </c>
       <c r="I3">
-        <v>10.19839163772356</v>
+        <v>34.25914524946653</v>
       </c>
       <c r="J3">
-        <v>6341912291.277191</v>
+        <v>6341012460.906618</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -562,13 +562,13 @@
         <v>15</v>
       </c>
       <c r="H4">
-        <v>6342368776.007891</v>
+        <v>6342375971.934543</v>
       </c>
       <c r="I4">
-        <v>10.19839163772356</v>
+        <v>34.25914524946653</v>
       </c>
       <c r="J4">
-        <v>6341912291.277191</v>
+        <v>6341012460.906618</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -594,13 +594,13 @@
         <v>16</v>
       </c>
       <c r="H5">
-        <v>6342368776.007891</v>
+        <v>6342375971.934543</v>
       </c>
       <c r="I5">
-        <v>10.19839163772356</v>
+        <v>34.25914524946653</v>
       </c>
       <c r="J5">
-        <v>6341912291.277191</v>
+        <v>6341012460.906618</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -626,13 +626,13 @@
         <v>17</v>
       </c>
       <c r="H6">
-        <v>6342368776.007891</v>
+        <v>6342375971.934543</v>
       </c>
       <c r="I6">
-        <v>10.19839163772356</v>
+        <v>34.25914524946653</v>
       </c>
       <c r="J6">
-        <v>6341912291.277191</v>
+        <v>6341012460.906618</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -658,13 +658,13 @@
         <v>18</v>
       </c>
       <c r="H7">
-        <v>6342368776.007891</v>
+        <v>6342375971.934543</v>
       </c>
       <c r="I7">
-        <v>10.19839163772356</v>
+        <v>34.25914524946653</v>
       </c>
       <c r="J7">
-        <v>6341912291.277191</v>
+        <v>6341012460.906618</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -690,13 +690,13 @@
         <v>19</v>
       </c>
       <c r="H8">
-        <v>6342368776.007891</v>
+        <v>6342375971.934543</v>
       </c>
       <c r="I8">
-        <v>10.19839163772356</v>
+        <v>34.25914524946653</v>
       </c>
       <c r="J8">
-        <v>6341912291.277191</v>
+        <v>6341012460.906618</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -722,13 +722,13 @@
         <v>20</v>
       </c>
       <c r="H9">
-        <v>6342368776.007891</v>
+        <v>6342375971.934543</v>
       </c>
       <c r="I9">
-        <v>10.19839163772356</v>
+        <v>34.25914524946653</v>
       </c>
       <c r="J9">
-        <v>6341912291.277191</v>
+        <v>6341012460.906618</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -754,13 +754,13 @@
         <v>21</v>
       </c>
       <c r="H10">
-        <v>6342368776.007891</v>
+        <v>6342375971.934543</v>
       </c>
       <c r="I10">
-        <v>10.19839163772356</v>
+        <v>34.25914524946653</v>
       </c>
       <c r="J10">
-        <v>6341912291.277191</v>
+        <v>6341012460.906618</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -786,13 +786,13 @@
         <v>22</v>
       </c>
       <c r="H11">
-        <v>6342368776.007891</v>
+        <v>6342375971.934543</v>
       </c>
       <c r="I11">
-        <v>10.19839163772356</v>
+        <v>34.25914524946653</v>
       </c>
       <c r="J11">
-        <v>6341912291.277191</v>
+        <v>6341012460.906618</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -818,13 +818,13 @@
         <v>13</v>
       </c>
       <c r="H12">
-        <v>6342521706.382955</v>
+        <v>6342576586.12755</v>
       </c>
       <c r="I12">
-        <v>10.48163318857942</v>
+        <v>34.10032615213645</v>
       </c>
       <c r="J12">
-        <v>6342061420.619566</v>
+        <v>6341219240.458123</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -850,13 +850,13 @@
         <v>14</v>
       </c>
       <c r="H13">
-        <v>6342368813.221176</v>
+        <v>6342376097.018803</v>
       </c>
       <c r="I13">
-        <v>10.18424946029083</v>
+        <v>34.14321232343269</v>
       </c>
       <c r="J13">
-        <v>6341913264.571548</v>
+        <v>6341019726.836246</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -882,13 +882,13 @@
         <v>15</v>
       </c>
       <c r="H14">
-        <v>6342405364.666583</v>
+        <v>6342423430.363872</v>
       </c>
       <c r="I14">
-        <v>10.17329617698618</v>
+        <v>34.036270160157</v>
       </c>
       <c r="J14">
-        <v>6341950275.284603</v>
+        <v>6341070559.121574</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -914,13 +914,13 @@
         <v>16</v>
       </c>
       <c r="H15">
-        <v>6342514276.112534</v>
+        <v>6342563908.649487</v>
       </c>
       <c r="I15">
-        <v>10.1875708224685</v>
+        <v>34.15083726685992</v>
       </c>
       <c r="J15">
-        <v>6342057368.509007</v>
+        <v>6341207384.261173</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -946,13 +946,13 @@
         <v>17</v>
       </c>
       <c r="H16">
-        <v>6342672469.884068</v>
+        <v>6342778033.797726</v>
       </c>
       <c r="I16">
-        <v>10.18246207501146</v>
+        <v>34.03090528548838</v>
       </c>
       <c r="J16">
-        <v>6342211394.151238</v>
+        <v>6341421849.574224</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -978,13 +978,13 @@
         <v>18</v>
       </c>
       <c r="H17">
-        <v>6342717648.899943</v>
+        <v>6342842797.599668</v>
       </c>
       <c r="I17">
-        <v>10.19644790625063</v>
+        <v>34.08844026641705</v>
       </c>
       <c r="J17">
-        <v>6342253190.36747</v>
+        <v>6341486538.314523</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1010,13 +1010,13 @@
         <v>19</v>
       </c>
       <c r="H18">
-        <v>6342645456.65773</v>
+        <v>6342740228.320789</v>
       </c>
       <c r="I18">
-        <v>10.24011958604608</v>
+        <v>34.06406869218731</v>
       </c>
       <c r="J18">
-        <v>6342175999.929125</v>
+        <v>6341382708.176293</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1042,13 +1042,13 @@
         <v>20</v>
       </c>
       <c r="H19">
-        <v>6342442033.71</v>
+        <v>6342473191.448194</v>
       </c>
       <c r="I19">
-        <v>10.35926697966381</v>
+        <v>34.12802685569632</v>
       </c>
       <c r="J19">
-        <v>6341977003.146873</v>
+        <v>6341113420.860023</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1074,13 +1074,13 @@
         <v>21</v>
       </c>
       <c r="H20">
-        <v>6342368792.750329</v>
+        <v>6342376020.508787</v>
       </c>
       <c r="I20">
-        <v>10.59200617078472</v>
+        <v>34.09145016467011</v>
       </c>
       <c r="J20">
-        <v>6341912820.229057</v>
+        <v>6341015420.181398</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1106,13 +1106,13 @@
         <v>22</v>
       </c>
       <c r="H21">
-        <v>6342368780.947937</v>
+        <v>6342375984.67053</v>
       </c>
       <c r="I21">
-        <v>11.79996460819718</v>
+        <v>34.24336211140866</v>
       </c>
       <c r="J21">
-        <v>6341912449.232902</v>
+        <v>6341013287.43663</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1138,13 +1138,13 @@
         <v>13</v>
       </c>
       <c r="H22">
-        <v>6342368776.007891</v>
+        <v>6342375971.934543</v>
       </c>
       <c r="I22">
-        <v>10.19839163772356</v>
+        <v>34.25914524946653</v>
       </c>
       <c r="J22">
-        <v>6330531182.982685</v>
+        <v>6302780251.74934</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1170,13 +1170,13 @@
         <v>14</v>
       </c>
       <c r="H23">
-        <v>6342368776.007891</v>
+        <v>6342375971.934543</v>
       </c>
       <c r="I23">
-        <v>10.19839163772356</v>
+        <v>34.25914524946653</v>
       </c>
       <c r="J23">
-        <v>6330531182.982685</v>
+        <v>6302780251.74934</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1202,13 +1202,13 @@
         <v>15</v>
       </c>
       <c r="H24">
-        <v>6342368776.007891</v>
+        <v>6342375971.934543</v>
       </c>
       <c r="I24">
-        <v>10.19839163772356</v>
+        <v>34.25914524946653</v>
       </c>
       <c r="J24">
-        <v>6330531182.982685</v>
+        <v>6302780251.74934</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1234,13 +1234,13 @@
         <v>16</v>
       </c>
       <c r="H25">
-        <v>6342368776.007891</v>
+        <v>6342375971.934543</v>
       </c>
       <c r="I25">
-        <v>10.19839163772356</v>
+        <v>34.25914524946653</v>
       </c>
       <c r="J25">
-        <v>6330531182.982685</v>
+        <v>6302780251.74934</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1266,13 +1266,13 @@
         <v>17</v>
       </c>
       <c r="H26">
-        <v>6342368776.007891</v>
+        <v>6342375971.934543</v>
       </c>
       <c r="I26">
-        <v>10.19839163772356</v>
+        <v>34.25914524946653</v>
       </c>
       <c r="J26">
-        <v>6330531182.982685</v>
+        <v>6302780251.74934</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1298,13 +1298,13 @@
         <v>18</v>
       </c>
       <c r="H27">
-        <v>6342368776.007891</v>
+        <v>6342375971.934543</v>
       </c>
       <c r="I27">
-        <v>10.19839163772356</v>
+        <v>34.25914524946653</v>
       </c>
       <c r="J27">
-        <v>6330531182.982685</v>
+        <v>6302780251.74934</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1330,13 +1330,13 @@
         <v>19</v>
       </c>
       <c r="H28">
-        <v>6342368776.007891</v>
+        <v>6342375971.934543</v>
       </c>
       <c r="I28">
-        <v>10.19839163772356</v>
+        <v>34.25914524946653</v>
       </c>
       <c r="J28">
-        <v>6330531182.982685</v>
+        <v>6302780251.74934</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1362,13 +1362,13 @@
         <v>20</v>
       </c>
       <c r="H29">
-        <v>6342368776.007891</v>
+        <v>6342375971.934543</v>
       </c>
       <c r="I29">
-        <v>10.19839163772356</v>
+        <v>34.25914524946653</v>
       </c>
       <c r="J29">
-        <v>6330531182.982685</v>
+        <v>6302780251.74934</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1394,13 +1394,13 @@
         <v>21</v>
       </c>
       <c r="H30">
-        <v>6342368776.007891</v>
+        <v>6342375971.934543</v>
       </c>
       <c r="I30">
-        <v>10.19839163772356</v>
+        <v>34.25914524946653</v>
       </c>
       <c r="J30">
-        <v>6330531182.982685</v>
+        <v>6302780251.74934</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1426,13 +1426,13 @@
         <v>22</v>
       </c>
       <c r="H31">
-        <v>6342368776.007891</v>
+        <v>6342375971.934543</v>
       </c>
       <c r="I31">
-        <v>10.19839163772356</v>
+        <v>34.25914524946653</v>
       </c>
       <c r="J31">
-        <v>6330531182.982685</v>
+        <v>6302780251.74934</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -1458,13 +1458,13 @@
         <v>13</v>
       </c>
       <c r="H32">
-        <v>6342521706.382955</v>
+        <v>6342576586.12755</v>
       </c>
       <c r="I32">
-        <v>10.48163318857942</v>
+        <v>34.10032615213645</v>
       </c>
       <c r="J32">
-        <v>6330364222.996638</v>
+        <v>6303164268.79183</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -1490,13 +1490,13 @@
         <v>14</v>
       </c>
       <c r="H33">
-        <v>6342368813.221176</v>
+        <v>6342376097.018803</v>
       </c>
       <c r="I33">
-        <v>10.18424946029083</v>
+        <v>34.14321232343269</v>
       </c>
       <c r="J33">
-        <v>6330547938.535522</v>
+        <v>6302916895.450773</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -1522,13 +1522,13 @@
         <v>15</v>
       </c>
       <c r="H34">
-        <v>6342405364.666583</v>
+        <v>6342423430.363872</v>
       </c>
       <c r="I34">
-        <v>10.17329617698618</v>
+        <v>34.036270160157</v>
       </c>
       <c r="J34">
-        <v>6330597172.794004</v>
+        <v>6303087072.0783</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -1554,13 +1554,13 @@
         <v>16</v>
       </c>
       <c r="H35">
-        <v>6342514276.112534</v>
+        <v>6342563908.649487</v>
       </c>
       <c r="I35">
-        <v>10.1875708224685</v>
+        <v>34.15083726685992</v>
       </c>
       <c r="J35">
-        <v>6330688335.929441</v>
+        <v>6303096043.660724</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -1586,13 +1586,13 @@
         <v>17</v>
       </c>
       <c r="H36">
-        <v>6342672469.884068</v>
+        <v>6342778033.797726</v>
       </c>
       <c r="I36">
-        <v>10.18246207501146</v>
+        <v>34.03090528548838</v>
       </c>
       <c r="J36">
-        <v>6330848062.785172</v>
+        <v>6303444349.574964</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -1618,13 +1618,13 @@
         <v>18</v>
       </c>
       <c r="H37">
-        <v>6342717648.899943</v>
+        <v>6342842797.599668</v>
       </c>
       <c r="I37">
-        <v>10.19644790625063</v>
+        <v>34.08844026641705</v>
       </c>
       <c r="J37">
-        <v>6330874251.220726</v>
+        <v>6303444830.950813</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -1650,13 +1650,13 @@
         <v>19</v>
       </c>
       <c r="H38">
-        <v>6342645456.65773</v>
+        <v>6342740228.320789</v>
       </c>
       <c r="I38">
-        <v>10.24011958604608</v>
+        <v>34.06406869218731</v>
       </c>
       <c r="J38">
-        <v>6330748324.458578</v>
+        <v>6303368198.780214</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -1682,13 +1682,13 @@
         <v>20</v>
       </c>
       <c r="H39">
-        <v>6342442033.71</v>
+        <v>6342473191.448194</v>
       </c>
       <c r="I39">
-        <v>10.35926697966381</v>
+        <v>34.12802685569632</v>
       </c>
       <c r="J39">
-        <v>6330416362.65224</v>
+        <v>6303027536.014648</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -1714,13 +1714,13 @@
         <v>21</v>
       </c>
       <c r="H40">
-        <v>6342368792.750329</v>
+        <v>6342376020.508787</v>
       </c>
       <c r="I40">
-        <v>10.59200617078472</v>
+        <v>34.09145016467011</v>
       </c>
       <c r="J40">
-        <v>6330092449.56984</v>
+        <v>6302970353.858827</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -1746,13 +1746,13 @@
         <v>22</v>
       </c>
       <c r="H41">
-        <v>6342368780.947937</v>
+        <v>6342375984.67053</v>
       </c>
       <c r="I41">
-        <v>11.79996460819718</v>
+        <v>34.24336211140866</v>
       </c>
       <c r="J41">
-        <v>6328744032.109124</v>
+        <v>6302798691.802134</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -1778,13 +1778,13 @@
         <v>13</v>
       </c>
       <c r="H42">
-        <v>6342368776.007891</v>
+        <v>6342375971.934543</v>
       </c>
       <c r="I42">
-        <v>10.19839163772356</v>
+        <v>34.25914524946653</v>
       </c>
       <c r="J42">
-        <v>6341912291.277191</v>
+        <v>6341012460.906618</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -1810,13 +1810,13 @@
         <v>14</v>
       </c>
       <c r="H43">
-        <v>6342368776.007891</v>
+        <v>6342375971.934543</v>
       </c>
       <c r="I43">
-        <v>10.19839163772356</v>
+        <v>34.25914524946653</v>
       </c>
       <c r="J43">
-        <v>6341912291.277191</v>
+        <v>6341012460.906618</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -1842,13 +1842,13 @@
         <v>15</v>
       </c>
       <c r="H44">
-        <v>6342368776.007891</v>
+        <v>6342375971.934543</v>
       </c>
       <c r="I44">
-        <v>10.19839163772356</v>
+        <v>34.25914524946653</v>
       </c>
       <c r="J44">
-        <v>6341912291.277191</v>
+        <v>6341012460.906618</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -1874,13 +1874,13 @@
         <v>16</v>
       </c>
       <c r="H45">
-        <v>6342368776.007891</v>
+        <v>6342375971.934543</v>
       </c>
       <c r="I45">
-        <v>10.19839163772356</v>
+        <v>34.25914524946653</v>
       </c>
       <c r="J45">
-        <v>6341912291.277191</v>
+        <v>6341012460.906618</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -1906,13 +1906,13 @@
         <v>17</v>
       </c>
       <c r="H46">
-        <v>6342368776.007891</v>
+        <v>6342375971.934543</v>
       </c>
       <c r="I46">
-        <v>10.19839163772356</v>
+        <v>34.25914524946653</v>
       </c>
       <c r="J46">
-        <v>6341912291.277191</v>
+        <v>6341012460.906618</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -1938,13 +1938,13 @@
         <v>18</v>
       </c>
       <c r="H47">
-        <v>6342368776.007891</v>
+        <v>6342375971.934543</v>
       </c>
       <c r="I47">
-        <v>10.19839163772356</v>
+        <v>34.25914524946653</v>
       </c>
       <c r="J47">
-        <v>6341912291.277191</v>
+        <v>6341012460.906618</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -1970,13 +1970,13 @@
         <v>19</v>
       </c>
       <c r="H48">
-        <v>6342368776.007891</v>
+        <v>6342375971.934543</v>
       </c>
       <c r="I48">
-        <v>10.19839163772356</v>
+        <v>34.25914524946653</v>
       </c>
       <c r="J48">
-        <v>6341912291.277191</v>
+        <v>6341012460.906618</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -2002,13 +2002,13 @@
         <v>20</v>
       </c>
       <c r="H49">
-        <v>6342368776.007891</v>
+        <v>6342375971.934543</v>
       </c>
       <c r="I49">
-        <v>10.19839163772356</v>
+        <v>34.25914524946653</v>
       </c>
       <c r="J49">
-        <v>6341912291.277191</v>
+        <v>6341012460.906618</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -2034,13 +2034,13 @@
         <v>21</v>
       </c>
       <c r="H50">
-        <v>6342368776.007891</v>
+        <v>6342375971.934543</v>
       </c>
       <c r="I50">
-        <v>10.19839163772356</v>
+        <v>34.25914524946653</v>
       </c>
       <c r="J50">
-        <v>6341912291.277191</v>
+        <v>6341012460.906618</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -2066,13 +2066,13 @@
         <v>22</v>
       </c>
       <c r="H51">
-        <v>6342368776.007891</v>
+        <v>6342375971.934543</v>
       </c>
       <c r="I51">
-        <v>10.19839163772356</v>
+        <v>34.25914524946653</v>
       </c>
       <c r="J51">
-        <v>6341912291.277191</v>
+        <v>6341012460.906618</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -2098,13 +2098,13 @@
         <v>13</v>
       </c>
       <c r="H52">
-        <v>6342521706.382955</v>
+        <v>6342576586.12755</v>
       </c>
       <c r="I52">
-        <v>10.48163318857942</v>
+        <v>34.10032615213645</v>
       </c>
       <c r="J52">
-        <v>6342061420.619566</v>
+        <v>6341219240.458123</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -2130,13 +2130,13 @@
         <v>14</v>
       </c>
       <c r="H53">
-        <v>6342368813.221176</v>
+        <v>6342376097.018803</v>
       </c>
       <c r="I53">
-        <v>10.18424946029083</v>
+        <v>34.14321232343269</v>
       </c>
       <c r="J53">
-        <v>6341913264.571548</v>
+        <v>6341019726.836246</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -2162,13 +2162,13 @@
         <v>15</v>
       </c>
       <c r="H54">
-        <v>6342405364.666583</v>
+        <v>6342423430.363872</v>
       </c>
       <c r="I54">
-        <v>10.17329617698618</v>
+        <v>34.036270160157</v>
       </c>
       <c r="J54">
-        <v>6341950275.284603</v>
+        <v>6341070559.121574</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -2194,13 +2194,13 @@
         <v>16</v>
       </c>
       <c r="H55">
-        <v>6342514276.112534</v>
+        <v>6342563908.649487</v>
       </c>
       <c r="I55">
-        <v>10.1875708224685</v>
+        <v>34.15083726685992</v>
       </c>
       <c r="J55">
-        <v>6342057368.509007</v>
+        <v>6341207384.261173</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -2226,13 +2226,13 @@
         <v>17</v>
       </c>
       <c r="H56">
-        <v>6342672469.884068</v>
+        <v>6342778033.797726</v>
       </c>
       <c r="I56">
-        <v>10.18246207501146</v>
+        <v>34.03090528548838</v>
       </c>
       <c r="J56">
-        <v>6342211394.151238</v>
+        <v>6341421849.574224</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -2258,13 +2258,13 @@
         <v>18</v>
       </c>
       <c r="H57">
-        <v>6342717648.899943</v>
+        <v>6342842797.599668</v>
       </c>
       <c r="I57">
-        <v>10.19644790625063</v>
+        <v>34.08844026641705</v>
       </c>
       <c r="J57">
-        <v>6342253190.36747</v>
+        <v>6341486538.314523</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -2290,13 +2290,13 @@
         <v>19</v>
       </c>
       <c r="H58">
-        <v>6342645456.65773</v>
+        <v>6342740228.320789</v>
       </c>
       <c r="I58">
-        <v>10.24011958604608</v>
+        <v>34.06406869218731</v>
       </c>
       <c r="J58">
-        <v>6342175999.929125</v>
+        <v>6341382708.176293</v>
       </c>
     </row>
     <row r="59" spans="1:10">
@@ -2322,13 +2322,13 @@
         <v>20</v>
       </c>
       <c r="H59">
-        <v>6342442033.71</v>
+        <v>6342473191.448194</v>
       </c>
       <c r="I59">
-        <v>10.35926697966381</v>
+        <v>34.12802685569632</v>
       </c>
       <c r="J59">
-        <v>6341977003.146873</v>
+        <v>6341113420.860023</v>
       </c>
     </row>
     <row r="60" spans="1:10">
@@ -2354,13 +2354,13 @@
         <v>21</v>
       </c>
       <c r="H60">
-        <v>6342368792.750329</v>
+        <v>6342376020.508787</v>
       </c>
       <c r="I60">
-        <v>10.59200617078472</v>
+        <v>34.09145016467011</v>
       </c>
       <c r="J60">
-        <v>6341912820.229057</v>
+        <v>6341015420.181398</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -2386,13 +2386,13 @@
         <v>22</v>
       </c>
       <c r="H61">
-        <v>6342368780.947937</v>
+        <v>6342375984.67053</v>
       </c>
       <c r="I61">
-        <v>11.79996460819718</v>
+        <v>34.24336211140866</v>
       </c>
       <c r="J61">
-        <v>6341912449.232902</v>
+        <v>6341013287.43663</v>
       </c>
     </row>
     <row r="62" spans="1:10">
@@ -2418,13 +2418,13 @@
         <v>13</v>
       </c>
       <c r="H62">
-        <v>6342368776.007891</v>
+        <v>6342375971.934543</v>
       </c>
       <c r="I62">
-        <v>10.19839163772356</v>
+        <v>34.25914524946653</v>
       </c>
       <c r="J62">
-        <v>6330531182.982685</v>
+        <v>6302780251.74934</v>
       </c>
     </row>
     <row r="63" spans="1:10">
@@ -2450,13 +2450,13 @@
         <v>14</v>
       </c>
       <c r="H63">
-        <v>6342368776.007891</v>
+        <v>6342375971.934543</v>
       </c>
       <c r="I63">
-        <v>10.19839163772356</v>
+        <v>34.25914524946653</v>
       </c>
       <c r="J63">
-        <v>6330531182.982685</v>
+        <v>6302780251.74934</v>
       </c>
     </row>
     <row r="64" spans="1:10">
@@ -2482,13 +2482,13 @@
         <v>15</v>
       </c>
       <c r="H64">
-        <v>6342368776.007891</v>
+        <v>6342375971.934543</v>
       </c>
       <c r="I64">
-        <v>10.19839163772356</v>
+        <v>34.25914524946653</v>
       </c>
       <c r="J64">
-        <v>6330531182.982685</v>
+        <v>6302780251.74934</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -2514,13 +2514,13 @@
         <v>16</v>
       </c>
       <c r="H65">
-        <v>6342368776.007891</v>
+        <v>6342375971.934543</v>
       </c>
       <c r="I65">
-        <v>10.19839163772356</v>
+        <v>34.25914524946653</v>
       </c>
       <c r="J65">
-        <v>6330531182.982685</v>
+        <v>6302780251.74934</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -2546,13 +2546,13 @@
         <v>17</v>
       </c>
       <c r="H66">
-        <v>6342368776.007891</v>
+        <v>6342375971.934543</v>
       </c>
       <c r="I66">
-        <v>10.19839163772356</v>
+        <v>34.25914524946653</v>
       </c>
       <c r="J66">
-        <v>6330531182.982685</v>
+        <v>6302780251.74934</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -2578,13 +2578,13 @@
         <v>18</v>
       </c>
       <c r="H67">
-        <v>6342368776.007891</v>
+        <v>6342375971.934543</v>
       </c>
       <c r="I67">
-        <v>10.19839163772356</v>
+        <v>34.25914524946653</v>
       </c>
       <c r="J67">
-        <v>6330531182.982685</v>
+        <v>6302780251.74934</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -2610,13 +2610,13 @@
         <v>19</v>
       </c>
       <c r="H68">
-        <v>6342368776.007891</v>
+        <v>6342375971.934543</v>
       </c>
       <c r="I68">
-        <v>10.19839163772356</v>
+        <v>34.25914524946653</v>
       </c>
       <c r="J68">
-        <v>6330531182.982685</v>
+        <v>6302780251.74934</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -2642,13 +2642,13 @@
         <v>20</v>
       </c>
       <c r="H69">
-        <v>6342368776.007891</v>
+        <v>6342375971.934543</v>
       </c>
       <c r="I69">
-        <v>10.19839163772356</v>
+        <v>34.25914524946653</v>
       </c>
       <c r="J69">
-        <v>6330531182.982685</v>
+        <v>6302780251.74934</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -2674,13 +2674,13 @@
         <v>21</v>
       </c>
       <c r="H70">
-        <v>6342368776.007891</v>
+        <v>6342375971.934543</v>
       </c>
       <c r="I70">
-        <v>10.19839163772356</v>
+        <v>34.25914524946653</v>
       </c>
       <c r="J70">
-        <v>6330531182.982685</v>
+        <v>6302780251.74934</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -2706,13 +2706,13 @@
         <v>22</v>
       </c>
       <c r="H71">
-        <v>6342368776.007891</v>
+        <v>6342375971.934543</v>
       </c>
       <c r="I71">
-        <v>10.19839163772356</v>
+        <v>34.25914524946653</v>
       </c>
       <c r="J71">
-        <v>6330531182.982685</v>
+        <v>6302780251.74934</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -2738,13 +2738,13 @@
         <v>13</v>
       </c>
       <c r="H72">
-        <v>6342521706.382955</v>
+        <v>6342576586.12755</v>
       </c>
       <c r="I72">
-        <v>10.48163318857942</v>
+        <v>34.10032615213645</v>
       </c>
       <c r="J72">
-        <v>6330364222.996638</v>
+        <v>6303164268.79183</v>
       </c>
     </row>
     <row r="73" spans="1:10">
@@ -2770,13 +2770,13 @@
         <v>14</v>
       </c>
       <c r="H73">
-        <v>6342368813.221176</v>
+        <v>6342376097.018803</v>
       </c>
       <c r="I73">
-        <v>10.18424946029083</v>
+        <v>34.14321232343269</v>
       </c>
       <c r="J73">
-        <v>6330547938.535522</v>
+        <v>6302916895.450773</v>
       </c>
     </row>
     <row r="74" spans="1:10">
@@ -2802,13 +2802,13 @@
         <v>15</v>
       </c>
       <c r="H74">
-        <v>6342405364.666583</v>
+        <v>6342423430.363872</v>
       </c>
       <c r="I74">
-        <v>10.17329617698618</v>
+        <v>34.036270160157</v>
       </c>
       <c r="J74">
-        <v>6330597172.794004</v>
+        <v>6303087072.0783</v>
       </c>
     </row>
     <row r="75" spans="1:10">
@@ -2834,13 +2834,13 @@
         <v>16</v>
       </c>
       <c r="H75">
-        <v>6342514276.112534</v>
+        <v>6342563908.649487</v>
       </c>
       <c r="I75">
-        <v>10.1875708224685</v>
+        <v>34.15083726685992</v>
       </c>
       <c r="J75">
-        <v>6330688335.929441</v>
+        <v>6303096043.660724</v>
       </c>
     </row>
     <row r="76" spans="1:10">
@@ -2866,13 +2866,13 @@
         <v>17</v>
       </c>
       <c r="H76">
-        <v>6342672469.884068</v>
+        <v>6342778033.797726</v>
       </c>
       <c r="I76">
-        <v>10.18246207501146</v>
+        <v>34.03090528548838</v>
       </c>
       <c r="J76">
-        <v>6330848062.785172</v>
+        <v>6303444349.574964</v>
       </c>
     </row>
     <row r="77" spans="1:10">
@@ -2898,13 +2898,13 @@
         <v>18</v>
       </c>
       <c r="H77">
-        <v>6342717648.899943</v>
+        <v>6342842797.599668</v>
       </c>
       <c r="I77">
-        <v>10.19644790625063</v>
+        <v>34.08844026641705</v>
       </c>
       <c r="J77">
-        <v>6330874251.220726</v>
+        <v>6303444830.950813</v>
       </c>
     </row>
     <row r="78" spans="1:10">
@@ -2930,13 +2930,13 @@
         <v>19</v>
       </c>
       <c r="H78">
-        <v>6342645456.65773</v>
+        <v>6342740228.320789</v>
       </c>
       <c r="I78">
-        <v>10.24011958604608</v>
+        <v>34.06406869218731</v>
       </c>
       <c r="J78">
-        <v>6330748324.458578</v>
+        <v>6303368198.780214</v>
       </c>
     </row>
     <row r="79" spans="1:10">
@@ -2962,13 +2962,13 @@
         <v>20</v>
       </c>
       <c r="H79">
-        <v>6342442033.71</v>
+        <v>6342473191.448194</v>
       </c>
       <c r="I79">
-        <v>10.35926697966381</v>
+        <v>34.12802685569632</v>
       </c>
       <c r="J79">
-        <v>6330416362.65224</v>
+        <v>6303027536.014648</v>
       </c>
     </row>
     <row r="80" spans="1:10">
@@ -2994,13 +2994,13 @@
         <v>21</v>
       </c>
       <c r="H80">
-        <v>6342368792.750329</v>
+        <v>6342376020.508787</v>
       </c>
       <c r="I80">
-        <v>10.59200617078472</v>
+        <v>34.09145016467011</v>
       </c>
       <c r="J80">
-        <v>6330092449.56984</v>
+        <v>6302970353.858827</v>
       </c>
     </row>
     <row r="81" spans="1:10">
@@ -3026,13 +3026,13 @@
         <v>22</v>
       </c>
       <c r="H81">
-        <v>6342368780.947937</v>
+        <v>6342375984.67053</v>
       </c>
       <c r="I81">
-        <v>11.79996460819718</v>
+        <v>34.24336211140866</v>
       </c>
       <c r="J81">
-        <v>6328744032.109124</v>
+        <v>6302798691.802134</v>
       </c>
     </row>
     <row r="82" spans="1:10">
@@ -3058,13 +3058,13 @@
         <v>13</v>
       </c>
       <c r="H82">
-        <v>3799741360.79353</v>
+        <v>3799773177.330956</v>
       </c>
       <c r="I82">
-        <v>10.15918104687676</v>
+        <v>34.10659875827898</v>
       </c>
       <c r="J82">
-        <v>3799286994.345078</v>
+        <v>3798415121.004986</v>
       </c>
     </row>
     <row r="83" spans="1:10">
@@ -3090,13 +3090,13 @@
         <v>14</v>
       </c>
       <c r="H83">
-        <v>3799741360.79353</v>
+        <v>3799773177.330956</v>
       </c>
       <c r="I83">
-        <v>10.15918104687676</v>
+        <v>34.10659875827898</v>
       </c>
       <c r="J83">
-        <v>3799286994.345078</v>
+        <v>3798415121.004986</v>
       </c>
     </row>
     <row r="84" spans="1:10">
@@ -3122,13 +3122,13 @@
         <v>15</v>
       </c>
       <c r="H84">
-        <v>3799741360.79353</v>
+        <v>3799773177.330956</v>
       </c>
       <c r="I84">
-        <v>10.15918104687676</v>
+        <v>34.10659875827898</v>
       </c>
       <c r="J84">
-        <v>3799286994.345078</v>
+        <v>3798415121.004986</v>
       </c>
     </row>
     <row r="85" spans="1:10">
@@ -3154,13 +3154,13 @@
         <v>16</v>
       </c>
       <c r="H85">
-        <v>3799741360.79353</v>
+        <v>3799773177.330956</v>
       </c>
       <c r="I85">
-        <v>10.15918104687676</v>
+        <v>34.10659875827898</v>
       </c>
       <c r="J85">
-        <v>3799286994.345078</v>
+        <v>3798415121.004986</v>
       </c>
     </row>
     <row r="86" spans="1:10">
@@ -3186,13 +3186,13 @@
         <v>17</v>
       </c>
       <c r="H86">
-        <v>3799741360.79353</v>
+        <v>3799773177.330956</v>
       </c>
       <c r="I86">
-        <v>10.15918104687676</v>
+        <v>34.10659875827898</v>
       </c>
       <c r="J86">
-        <v>3799286994.345078</v>
+        <v>3798415121.004986</v>
       </c>
     </row>
     <row r="87" spans="1:10">
@@ -3218,13 +3218,13 @@
         <v>18</v>
       </c>
       <c r="H87">
-        <v>3799741360.79353</v>
+        <v>3799773177.330956</v>
       </c>
       <c r="I87">
-        <v>10.15918104687676</v>
+        <v>34.10659875827898</v>
       </c>
       <c r="J87">
-        <v>3799286994.345078</v>
+        <v>3798415121.004986</v>
       </c>
     </row>
     <row r="88" spans="1:10">
@@ -3250,13 +3250,13 @@
         <v>19</v>
       </c>
       <c r="H88">
-        <v>3799741360.79353</v>
+        <v>3799773177.330956</v>
       </c>
       <c r="I88">
-        <v>10.15918104687676</v>
+        <v>34.10659875827898</v>
       </c>
       <c r="J88">
-        <v>3799286994.345078</v>
+        <v>3798415121.004986</v>
       </c>
     </row>
     <row r="89" spans="1:10">
@@ -3282,13 +3282,13 @@
         <v>20</v>
       </c>
       <c r="H89">
-        <v>3799741360.79353</v>
+        <v>3799773177.330956</v>
       </c>
       <c r="I89">
-        <v>10.15918104687676</v>
+        <v>34.10659875827898</v>
       </c>
       <c r="J89">
-        <v>3799286994.345078</v>
+        <v>3798415121.004986</v>
       </c>
     </row>
     <row r="90" spans="1:10">
@@ -3314,13 +3314,13 @@
         <v>21</v>
       </c>
       <c r="H90">
-        <v>3799741360.79353</v>
+        <v>3799773177.330956</v>
       </c>
       <c r="I90">
-        <v>10.15918104687676</v>
+        <v>34.10659875827898</v>
       </c>
       <c r="J90">
-        <v>3799286994.345078</v>
+        <v>3798415121.004986</v>
       </c>
     </row>
     <row r="91" spans="1:10">
@@ -3346,13 +3346,13 @@
         <v>22</v>
       </c>
       <c r="H91">
-        <v>3799741360.79353</v>
+        <v>3799773177.330956</v>
       </c>
       <c r="I91">
-        <v>10.15918104687676</v>
+        <v>34.10659875827898</v>
       </c>
       <c r="J91">
-        <v>3799286994.345078</v>
+        <v>3798415121.004986</v>
       </c>
     </row>
     <row r="92" spans="1:10">
@@ -3378,13 +3378,13 @@
         <v>13</v>
       </c>
       <c r="H92">
-        <v>3799948345.855133</v>
+        <v>3800034567.568944</v>
       </c>
       <c r="I92">
-        <v>10.43986102682867</v>
+        <v>33.94946948642339</v>
       </c>
       <c r="J92">
-        <v>3799490191.116305</v>
+        <v>3798682615.917453</v>
       </c>
     </row>
     <row r="93" spans="1:10">
@@ -3410,13 +3410,13 @@
         <v>14</v>
       </c>
       <c r="H93">
-        <v>3799741367.210475</v>
+        <v>3799773130.948736</v>
       </c>
       <c r="I93">
-        <v>10.14514777280499</v>
+        <v>33.99122071429865</v>
       </c>
       <c r="J93">
-        <v>3799287929.23979</v>
+        <v>3798422187.491334</v>
       </c>
     </row>
     <row r="94" spans="1:10">
@@ -3442,13 +3442,13 @@
         <v>15</v>
       </c>
       <c r="H94">
-        <v>3799790804.821797</v>
+        <v>3799834807.697386</v>
       </c>
       <c r="I94">
-        <v>10.13441996662276</v>
+        <v>33.88532941006384</v>
       </c>
       <c r="J94">
-        <v>3799337817.057675</v>
+        <v>3798487338.348712</v>
       </c>
     </row>
     <row r="95" spans="1:10">
@@ -3474,13 +3474,13 @@
         <v>16</v>
       </c>
       <c r="H95">
-        <v>3799937754.736739</v>
+        <v>3800017878.389256</v>
       </c>
       <c r="I95">
-        <v>10.14868985283323</v>
+        <v>33.99969777679402</v>
       </c>
       <c r="J95">
-        <v>3799482945.282347</v>
+        <v>3798666719.576719</v>
       </c>
     </row>
     <row r="96" spans="1:10">
@@ -3506,13 +3506,13 @@
         <v>17</v>
       </c>
       <c r="H96">
-        <v>3800153360.872786</v>
+        <v>3800297791.326332</v>
       </c>
       <c r="I96">
-        <v>10.14370282544296</v>
+        <v>33.8804865837351</v>
       </c>
       <c r="J96">
-        <v>3799694413.956134</v>
+        <v>3798946959.327835</v>
       </c>
     </row>
     <row r="97" spans="1:10">
@@ -3538,13 +3538,13 @@
         <v>18</v>
       </c>
       <c r="H97">
-        <v>3800215882.916114</v>
+        <v>3800382653.053405</v>
       </c>
       <c r="I97">
-        <v>10.15863234906188</v>
+        <v>33.94171031669325</v>
       </c>
       <c r="J97">
-        <v>3799753576.485013</v>
+        <v>3799031727.671643</v>
       </c>
     </row>
     <row r="98" spans="1:10">
@@ -3570,13 +3570,13 @@
         <v>19</v>
       </c>
       <c r="H98">
-        <v>3800117508.55275</v>
+        <v>3800248663.859992</v>
       </c>
       <c r="I98">
-        <v>10.20081054533517</v>
+        <v>33.91316149838278</v>
       </c>
       <c r="J98">
-        <v>3799650257.834416</v>
+        <v>3798896521.444519</v>
       </c>
     </row>
     <row r="99" spans="1:10">
@@ -3602,13 +3602,13 @@
         <v>20</v>
       </c>
       <c r="H99">
-        <v>3799841767.311872</v>
+        <v>3799900431.854399</v>
       </c>
       <c r="I99">
-        <v>10.31946676923278</v>
+        <v>33.97602563082212</v>
       </c>
       <c r="J99">
-        <v>3799378886.473526</v>
+        <v>3798546095.553426</v>
       </c>
     </row>
     <row r="100" spans="1:10">
@@ -3634,13 +3634,13 @@
         <v>21</v>
       </c>
       <c r="H100">
-        <v>3799741363.412524</v>
+        <v>3799773156.992503</v>
       </c>
       <c r="I100">
-        <v>10.55094251494497</v>
+        <v>33.93955537195189</v>
       </c>
       <c r="J100">
-        <v>3799287500.972907</v>
+        <v>3798417992.249275</v>
       </c>
     </row>
     <row r="101" spans="1:10">
@@ -3666,13 +3666,13 @@
         <v>22</v>
       </c>
       <c r="H101">
-        <v>3799741361.432154</v>
+        <v>3799773170.423244</v>
       </c>
       <c r="I101">
-        <v>11.74086178827164</v>
+        <v>34.09100822595038</v>
       </c>
       <c r="J101">
-        <v>3799287142.933431</v>
+        <v>3798415915.789246</v>
       </c>
     </row>
     <row r="102" spans="1:10">
@@ -3698,13 +3698,13 @@
         <v>13</v>
       </c>
       <c r="H102">
-        <v>3799741360.79353</v>
+        <v>3799773177.330956</v>
       </c>
       <c r="I102">
-        <v>10.15918104687676</v>
+        <v>34.10659875827898</v>
       </c>
       <c r="J102">
-        <v>3787949643.928932</v>
+        <v>3760353149.29277</v>
       </c>
     </row>
     <row r="103" spans="1:10">
@@ -3730,13 +3730,13 @@
         <v>14</v>
       </c>
       <c r="H103">
-        <v>3799741360.79353</v>
+        <v>3799773177.330956</v>
       </c>
       <c r="I103">
-        <v>10.15918104687676</v>
+        <v>34.10659875827898</v>
       </c>
       <c r="J103">
-        <v>3787949643.928932</v>
+        <v>3760353149.29277</v>
       </c>
     </row>
     <row r="104" spans="1:10">
@@ -3762,13 +3762,13 @@
         <v>15</v>
       </c>
       <c r="H104">
-        <v>3799741360.79353</v>
+        <v>3799773177.330956</v>
       </c>
       <c r="I104">
-        <v>10.15918104687676</v>
+        <v>34.10659875827898</v>
       </c>
       <c r="J104">
-        <v>3787949643.928932</v>
+        <v>3760353149.29277</v>
       </c>
     </row>
     <row r="105" spans="1:10">
@@ -3794,13 +3794,13 @@
         <v>16</v>
       </c>
       <c r="H105">
-        <v>3799741360.79353</v>
+        <v>3799773177.330956</v>
       </c>
       <c r="I105">
-        <v>10.15918104687676</v>
+        <v>34.10659875827898</v>
       </c>
       <c r="J105">
-        <v>3787949643.928932</v>
+        <v>3760353149.29277</v>
       </c>
     </row>
     <row r="106" spans="1:10">
@@ -3826,13 +3826,13 @@
         <v>17</v>
       </c>
       <c r="H106">
-        <v>3799741360.79353</v>
+        <v>3799773177.330956</v>
       </c>
       <c r="I106">
-        <v>10.15918104687676</v>
+        <v>34.10659875827898</v>
       </c>
       <c r="J106">
-        <v>3787949643.928932</v>
+        <v>3760353149.29277</v>
       </c>
     </row>
     <row r="107" spans="1:10">
@@ -3858,13 +3858,13 @@
         <v>18</v>
       </c>
       <c r="H107">
-        <v>3799741360.79353</v>
+        <v>3799773177.330956</v>
       </c>
       <c r="I107">
-        <v>10.15918104687676</v>
+        <v>34.10659875827898</v>
       </c>
       <c r="J107">
-        <v>3787949643.928932</v>
+        <v>3760353149.29277</v>
       </c>
     </row>
     <row r="108" spans="1:10">
@@ -3890,13 +3890,13 @@
         <v>19</v>
       </c>
       <c r="H108">
-        <v>3799741360.79353</v>
+        <v>3799773177.330956</v>
       </c>
       <c r="I108">
-        <v>10.15918104687676</v>
+        <v>34.10659875827898</v>
       </c>
       <c r="J108">
-        <v>3787949643.928932</v>
+        <v>3760353149.29277</v>
       </c>
     </row>
     <row r="109" spans="1:10">
@@ -3922,13 +3922,13 @@
         <v>20</v>
       </c>
       <c r="H109">
-        <v>3799741360.79353</v>
+        <v>3799773177.330956</v>
       </c>
       <c r="I109">
-        <v>10.15918104687676</v>
+        <v>34.10659875827898</v>
       </c>
       <c r="J109">
-        <v>3787949643.928932</v>
+        <v>3760353149.29277</v>
       </c>
     </row>
     <row r="110" spans="1:10">
@@ -3954,13 +3954,13 @@
         <v>21</v>
       </c>
       <c r="H110">
-        <v>3799741360.79353</v>
+        <v>3799773177.330956</v>
       </c>
       <c r="I110">
-        <v>10.15918104687676</v>
+        <v>34.10659875827898</v>
       </c>
       <c r="J110">
-        <v>3787949643.928932</v>
+        <v>3760353149.29277</v>
       </c>
     </row>
     <row r="111" spans="1:10">
@@ -3986,13 +3986,13 @@
         <v>22</v>
       </c>
       <c r="H111">
-        <v>3799741360.79353</v>
+        <v>3799773177.330956</v>
       </c>
       <c r="I111">
-        <v>10.15918104687676</v>
+        <v>34.10659875827898</v>
       </c>
       <c r="J111">
-        <v>3787949643.928932</v>
+        <v>3760353149.29277</v>
       </c>
     </row>
     <row r="112" spans="1:10">
@@ -4018,13 +4018,13 @@
         <v>13</v>
       </c>
       <c r="H112">
-        <v>3799948345.855133</v>
+        <v>3800034567.568944</v>
       </c>
       <c r="I112">
-        <v>10.43986102682867</v>
+        <v>33.94946948642339</v>
       </c>
       <c r="J112">
-        <v>3787839610.01032</v>
+        <v>3760795995.900167</v>
       </c>
     </row>
     <row r="113" spans="1:10">
@@ -4050,13 +4050,13 @@
         <v>14</v>
       </c>
       <c r="H113">
-        <v>3799741367.210475</v>
+        <v>3799773130.948736</v>
       </c>
       <c r="I113">
-        <v>10.14514777280499</v>
+        <v>33.99122071429865</v>
       </c>
       <c r="J113">
-        <v>3787966239.54914</v>
+        <v>3760488974.318699</v>
       </c>
     </row>
     <row r="114" spans="1:10">
@@ -4082,13 +4082,13 @@
         <v>15</v>
       </c>
       <c r="H114">
-        <v>3799790804.821797</v>
+        <v>3799834807.697386</v>
       </c>
       <c r="I114">
-        <v>10.13441996662276</v>
+        <v>33.88532941006384</v>
       </c>
       <c r="J114">
-        <v>3788028099.286545</v>
+        <v>3760672296.790166</v>
       </c>
     </row>
     <row r="115" spans="1:10">
@@ -4114,13 +4114,13 @@
         <v>16</v>
       </c>
       <c r="H115">
-        <v>3799937754.736739</v>
+        <v>3800017878.389256</v>
       </c>
       <c r="I115">
-        <v>10.14868985283323</v>
+        <v>33.99969777679402</v>
       </c>
       <c r="J115">
-        <v>3788157302.73346</v>
+        <v>3760724046.249022</v>
       </c>
     </row>
     <row r="116" spans="1:10">
@@ -4146,13 +4146,13 @@
         <v>17</v>
       </c>
       <c r="H116">
-        <v>3800153360.872786</v>
+        <v>3800297791.326332</v>
       </c>
       <c r="I116">
-        <v>10.14370282544296</v>
+        <v>33.8804865837351</v>
       </c>
       <c r="J116">
-        <v>3788374336.784692</v>
+        <v>3761137322.222546</v>
       </c>
     </row>
     <row r="117" spans="1:10">
@@ -4178,13 +4178,13 @@
         <v>18</v>
       </c>
       <c r="H117">
-        <v>3800215882.916114</v>
+        <v>3800382653.053405</v>
       </c>
       <c r="I117">
-        <v>10.15863234906188</v>
+        <v>33.94171031669325</v>
       </c>
       <c r="J117">
-        <v>3788416838.39966</v>
+        <v>3761153766.661984</v>
       </c>
     </row>
     <row r="118" spans="1:10">
@@ -4210,13 +4210,13 @@
         <v>19</v>
       </c>
       <c r="H118">
-        <v>3800117508.55275</v>
+        <v>3800248663.859992</v>
       </c>
       <c r="I118">
-        <v>10.20081054533517</v>
+        <v>33.91316149838278</v>
       </c>
       <c r="J118">
-        <v>3788266450.109409</v>
+        <v>3761050420.085324</v>
       </c>
     </row>
     <row r="119" spans="1:10">
@@ -4242,13 +4242,13 @@
         <v>20</v>
       </c>
       <c r="H119">
-        <v>3799841767.311872</v>
+        <v>3799900431.854399</v>
       </c>
       <c r="I119">
-        <v>10.31946676923278</v>
+        <v>33.97602563082212</v>
       </c>
       <c r="J119">
-        <v>3787862661.855545</v>
+        <v>3760629839.651773</v>
       </c>
     </row>
     <row r="120" spans="1:10">
@@ -4274,13 +4274,13 @@
         <v>21</v>
       </c>
       <c r="H120">
-        <v>3799741363.412524</v>
+        <v>3799773156.992503</v>
       </c>
       <c r="I120">
-        <v>10.55094251494497</v>
+        <v>33.93955537195189</v>
       </c>
       <c r="J120">
-        <v>3787512956.158654</v>
+        <v>3760542436.095238</v>
       </c>
     </row>
     <row r="121" spans="1:10">
@@ -4306,13 +4306,13 @@
         <v>22</v>
       </c>
       <c r="H121">
-        <v>3799741361.432154</v>
+        <v>3799773170.423244</v>
       </c>
       <c r="I121">
-        <v>11.74086178827164</v>
+        <v>34.09100822595038</v>
       </c>
       <c r="J121">
-        <v>3786184682.836796</v>
+        <v>3760371342.657423</v>
       </c>
     </row>
     <row r="122" spans="1:10">
@@ -4338,13 +4338,13 @@
         <v>13</v>
       </c>
       <c r="H122">
-        <v>15292117296.87737</v>
+        <v>15290931613.23288</v>
       </c>
       <c r="I122">
-        <v>24.06418337369001</v>
+        <v>338.3752225493016</v>
       </c>
       <c r="J122">
-        <v>15290967147.68263</v>
+        <v>15278490664.85824</v>
       </c>
     </row>
     <row r="123" spans="1:10">
@@ -4370,13 +4370,13 @@
         <v>14</v>
       </c>
       <c r="H123">
-        <v>15292117296.87737</v>
+        <v>15290931613.23288</v>
       </c>
       <c r="I123">
-        <v>24.06418337369001</v>
+        <v>338.3752225493016</v>
       </c>
       <c r="J123">
-        <v>15290967147.68263</v>
+        <v>15278490664.85824</v>
       </c>
     </row>
     <row r="124" spans="1:10">
@@ -4402,13 +4402,13 @@
         <v>15</v>
       </c>
       <c r="H124">
-        <v>15292117296.87737</v>
+        <v>15290931613.23288</v>
       </c>
       <c r="I124">
-        <v>24.06418337369001</v>
+        <v>338.3752225493016</v>
       </c>
       <c r="J124">
-        <v>15290967147.68263</v>
+        <v>15278490664.85824</v>
       </c>
     </row>
     <row r="125" spans="1:10">
@@ -4434,13 +4434,13 @@
         <v>16</v>
       </c>
       <c r="H125">
-        <v>15292117296.87737</v>
+        <v>15290931613.23288</v>
       </c>
       <c r="I125">
-        <v>24.06418337369001</v>
+        <v>338.3752225493016</v>
       </c>
       <c r="J125">
-        <v>15290967147.68263</v>
+        <v>15278490664.85824</v>
       </c>
     </row>
     <row r="126" spans="1:10">
@@ -4466,13 +4466,13 @@
         <v>17</v>
       </c>
       <c r="H126">
-        <v>15292117296.87737</v>
+        <v>15290931613.23288</v>
       </c>
       <c r="I126">
-        <v>24.06418337369001</v>
+        <v>338.3752225493016</v>
       </c>
       <c r="J126">
-        <v>15290967147.68263</v>
+        <v>15278490664.85824</v>
       </c>
     </row>
     <row r="127" spans="1:10">
@@ -4498,13 +4498,13 @@
         <v>18</v>
       </c>
       <c r="H127">
-        <v>15292117296.87737</v>
+        <v>15290931613.23288</v>
       </c>
       <c r="I127">
-        <v>24.06418337369001</v>
+        <v>338.3752225493016</v>
       </c>
       <c r="J127">
-        <v>15290967147.68263</v>
+        <v>15278490664.85824</v>
       </c>
     </row>
     <row r="128" spans="1:10">
@@ -4530,13 +4530,13 @@
         <v>19</v>
       </c>
       <c r="H128">
-        <v>15292117296.87737</v>
+        <v>15290931613.23288</v>
       </c>
       <c r="I128">
-        <v>24.06418337369001</v>
+        <v>338.3752225493016</v>
       </c>
       <c r="J128">
-        <v>15290967147.68263</v>
+        <v>15278490664.85824</v>
       </c>
     </row>
     <row r="129" spans="1:10">
@@ -4562,13 +4562,13 @@
         <v>20</v>
       </c>
       <c r="H129">
-        <v>15292117296.87737</v>
+        <v>15290931613.23288</v>
       </c>
       <c r="I129">
-        <v>24.06418337369001</v>
+        <v>338.3752225493016</v>
       </c>
       <c r="J129">
-        <v>15290967147.68263</v>
+        <v>15278490664.85824</v>
       </c>
     </row>
     <row r="130" spans="1:10">
@@ -4594,13 +4594,13 @@
         <v>21</v>
       </c>
       <c r="H130">
-        <v>15292117296.87737</v>
+        <v>15290931613.23288</v>
       </c>
       <c r="I130">
-        <v>24.06418337369001</v>
+        <v>338.3752225493016</v>
       </c>
       <c r="J130">
-        <v>15290967147.68263</v>
+        <v>15278490664.85824</v>
       </c>
     </row>
     <row r="131" spans="1:10">
@@ -4626,13 +4626,13 @@
         <v>22</v>
       </c>
       <c r="H131">
-        <v>15292117296.87737</v>
+        <v>15290931613.23288</v>
       </c>
       <c r="I131">
-        <v>24.06418337369001</v>
+        <v>338.3752225493016</v>
       </c>
       <c r="J131">
-        <v>15290967147.68263</v>
+        <v>15278490664.85824</v>
       </c>
     </row>
     <row r="132" spans="1:10">
@@ -4658,13 +4658,13 @@
         <v>13</v>
       </c>
       <c r="H132">
-        <v>15291905756.58414</v>
+        <v>15290664202.02018</v>
       </c>
       <c r="I132">
-        <v>24.85959982315621</v>
+        <v>333.6249040370462</v>
       </c>
       <c r="J132">
-        <v>15290751425.84189</v>
+        <v>15278391331.20192</v>
       </c>
     </row>
     <row r="133" spans="1:10">
@@ -4690,13 +4690,13 @@
         <v>14</v>
       </c>
       <c r="H133">
-        <v>15292118130.27146</v>
+        <v>15290942289.12078</v>
       </c>
       <c r="I133">
-        <v>23.9713239913244</v>
+        <v>336.2891175793375</v>
       </c>
       <c r="J133">
-        <v>15290973523.95151</v>
+        <v>15278596308.38635</v>
       </c>
     </row>
     <row r="134" spans="1:10">
@@ -4722,13 +4722,13 @@
         <v>15</v>
       </c>
       <c r="H134">
-        <v>15292072871.26419</v>
+        <v>15290899965.69983</v>
       </c>
       <c r="I134">
-        <v>23.8150398963533</v>
+        <v>331.9518071295795</v>
       </c>
       <c r="J134">
-        <v>15290936697.07932</v>
+        <v>15278727615.38073</v>
       </c>
     </row>
     <row r="135" spans="1:10">
@@ -4754,13 +4754,13 @@
         <v>16</v>
       </c>
       <c r="H135">
-        <v>15291893158.8806</v>
+        <v>15290646434.90685</v>
       </c>
       <c r="I135">
-        <v>23.86960169517343</v>
+        <v>333.1998288522125</v>
       </c>
       <c r="J135">
-        <v>15290751482.84371</v>
+        <v>15278446791.82243</v>
       </c>
     </row>
     <row r="136" spans="1:10">
@@ -4786,13 +4786,13 @@
         <v>17</v>
       </c>
       <c r="H136">
-        <v>15291666255.03229</v>
+        <v>15290337357.97599</v>
       </c>
       <c r="I136">
-        <v>23.84461676080356</v>
+        <v>332.5551969767691</v>
       </c>
       <c r="J136">
-        <v>15290512663.87971</v>
+        <v>15278132528.61247</v>
       </c>
     </row>
     <row r="137" spans="1:10">
@@ -4818,13 +4818,13 @@
         <v>18</v>
       </c>
       <c r="H137">
-        <v>15291615479.89652</v>
+        <v>15290266855.62614</v>
       </c>
       <c r="I137">
-        <v>23.76398214001628</v>
+        <v>330.4240721488735</v>
       </c>
       <c r="J137">
-        <v>15290452880.987</v>
+        <v>15278049715.54913</v>
       </c>
     </row>
     <row r="138" spans="1:10">
@@ -4850,13 +4850,13 @@
         <v>19</v>
       </c>
       <c r="H138">
-        <v>15291677523.23417</v>
+        <v>15290342605.2949</v>
       </c>
       <c r="I138">
-        <v>24.01597539409756</v>
+        <v>332.9994023761273</v>
       </c>
       <c r="J138">
-        <v>15290494575.82631</v>
+        <v>15278081758.65718</v>
       </c>
     </row>
     <row r="139" spans="1:10">
@@ -4882,13 +4882,13 @@
         <v>20</v>
       </c>
       <c r="H139">
-        <v>15291995874.36903</v>
+        <v>15290774012.84996</v>
       </c>
       <c r="I139">
-        <v>24.41367285126583</v>
+        <v>334.7719959555027</v>
       </c>
       <c r="J139">
-        <v>15290823649.79579</v>
+        <v>15278424493.69379</v>
       </c>
     </row>
     <row r="140" spans="1:10">
@@ -4914,13 +4914,13 @@
         <v>21</v>
       </c>
       <c r="H140">
-        <v>15292118157.63056</v>
+        <v>15290941153.21388</v>
       </c>
       <c r="I140">
-        <v>25.18432046828665</v>
+        <v>335.2656000182092</v>
       </c>
       <c r="J140">
-        <v>15290974396.22249</v>
+        <v>15278587546.81272</v>
       </c>
     </row>
     <row r="141" spans="1:10">
@@ -4946,13 +4946,13 @@
         <v>22</v>
       </c>
       <c r="H141">
-        <v>15292117576.09421</v>
+        <v>15290934870.8301</v>
       </c>
       <c r="I141">
-        <v>29.82984208280117</v>
+        <v>336.9025321004047</v>
       </c>
       <c r="J141">
-        <v>15290969432.01127</v>
+        <v>15278523104.5774</v>
       </c>
     </row>
     <row r="142" spans="1:10">
@@ -4978,13 +4978,13 @@
         <v>13</v>
       </c>
       <c r="H142">
-        <v>15292117296.87737</v>
+        <v>15290931613.23288</v>
       </c>
       <c r="I142">
-        <v>24.06418337369001</v>
+        <v>338.3752225493016</v>
       </c>
       <c r="J142">
-        <v>15264112219.30532</v>
+        <v>14900873763.2122</v>
       </c>
     </row>
     <row r="143" spans="1:10">
@@ -5010,13 +5010,13 @@
         <v>14</v>
       </c>
       <c r="H143">
-        <v>15292117296.87737</v>
+        <v>15290931613.23288</v>
       </c>
       <c r="I143">
-        <v>24.06418337369001</v>
+        <v>338.3752225493016</v>
       </c>
       <c r="J143">
-        <v>15264112219.30532</v>
+        <v>14900873763.2122</v>
       </c>
     </row>
     <row r="144" spans="1:10">
@@ -5042,13 +5042,13 @@
         <v>15</v>
       </c>
       <c r="H144">
-        <v>15292117296.87737</v>
+        <v>15290931613.23288</v>
       </c>
       <c r="I144">
-        <v>24.06418337369001</v>
+        <v>338.3752225493016</v>
       </c>
       <c r="J144">
-        <v>15264112219.30532</v>
+        <v>14900873763.2122</v>
       </c>
     </row>
     <row r="145" spans="1:10">
@@ -5074,13 +5074,13 @@
         <v>16</v>
       </c>
       <c r="H145">
-        <v>15292117296.87737</v>
+        <v>15290931613.23288</v>
       </c>
       <c r="I145">
-        <v>24.06418337369001</v>
+        <v>338.3752225493016</v>
       </c>
       <c r="J145">
-        <v>15264112219.30532</v>
+        <v>14900873763.2122</v>
       </c>
     </row>
     <row r="146" spans="1:10">
@@ -5106,13 +5106,13 @@
         <v>17</v>
       </c>
       <c r="H146">
-        <v>15292117296.87737</v>
+        <v>15290931613.23288</v>
       </c>
       <c r="I146">
-        <v>24.06418337369001</v>
+        <v>338.3752225493016</v>
       </c>
       <c r="J146">
-        <v>15264112219.30532</v>
+        <v>14900873763.2122</v>
       </c>
     </row>
     <row r="147" spans="1:10">
@@ -5138,13 +5138,13 @@
         <v>18</v>
       </c>
       <c r="H147">
-        <v>15292117296.87737</v>
+        <v>15290931613.23288</v>
       </c>
       <c r="I147">
-        <v>24.06418337369001</v>
+        <v>338.3752225493016</v>
       </c>
       <c r="J147">
-        <v>15264112219.30532</v>
+        <v>14900873763.2122</v>
       </c>
     </row>
     <row r="148" spans="1:10">
@@ -5170,13 +5170,13 @@
         <v>19</v>
       </c>
       <c r="H148">
-        <v>15292117296.87737</v>
+        <v>15290931613.23288</v>
       </c>
       <c r="I148">
-        <v>24.06418337369001</v>
+        <v>338.3752225493016</v>
       </c>
       <c r="J148">
-        <v>15264112219.30532</v>
+        <v>14900873763.2122</v>
       </c>
     </row>
     <row r="149" spans="1:10">
@@ -5202,13 +5202,13 @@
         <v>20</v>
       </c>
       <c r="H149">
-        <v>15292117296.87737</v>
+        <v>15290931613.23288</v>
       </c>
       <c r="I149">
-        <v>24.06418337369001</v>
+        <v>338.3752225493016</v>
       </c>
       <c r="J149">
-        <v>15264112219.30532</v>
+        <v>14900873763.2122</v>
       </c>
     </row>
     <row r="150" spans="1:10">
@@ -5234,13 +5234,13 @@
         <v>21</v>
       </c>
       <c r="H150">
-        <v>15292117296.87737</v>
+        <v>15290931613.23288</v>
       </c>
       <c r="I150">
-        <v>24.06418337369001</v>
+        <v>338.3752225493016</v>
       </c>
       <c r="J150">
-        <v>15264112219.30532</v>
+        <v>14900873763.2122</v>
       </c>
     </row>
     <row r="151" spans="1:10">
@@ -5266,13 +5266,13 @@
         <v>22</v>
       </c>
       <c r="H151">
-        <v>15292117296.87737</v>
+        <v>15290931613.23288</v>
       </c>
       <c r="I151">
-        <v>24.06418337369001</v>
+        <v>338.3752225493016</v>
       </c>
       <c r="J151">
-        <v>15264112219.30532</v>
+        <v>14900873763.2122</v>
       </c>
     </row>
     <row r="152" spans="1:10">
@@ -5298,13 +5298,13 @@
         <v>13</v>
       </c>
       <c r="H152">
-        <v>15291905756.58414</v>
+        <v>15290664202.02018</v>
       </c>
       <c r="I152">
-        <v>24.85959982315621</v>
+        <v>333.6249040370462</v>
       </c>
       <c r="J152">
-        <v>15263008835.85361</v>
+        <v>14906075646.78129</v>
       </c>
     </row>
     <row r="153" spans="1:10">
@@ -5330,13 +5330,13 @@
         <v>14</v>
       </c>
       <c r="H153">
-        <v>15292118130.27146</v>
+        <v>15290942289.12078</v>
       </c>
       <c r="I153">
-        <v>23.9713239913244</v>
+        <v>336.2891175793375</v>
       </c>
       <c r="J153">
-        <v>15264222223.94272</v>
+        <v>14903307439.18113</v>
       </c>
     </row>
     <row r="154" spans="1:10">
@@ -5362,13 +5362,13 @@
         <v>15</v>
       </c>
       <c r="H154">
-        <v>15292072871.26419</v>
+        <v>15290899965.69983</v>
       </c>
       <c r="I154">
-        <v>23.8150398963533</v>
+        <v>331.9518071295795</v>
       </c>
       <c r="J154">
-        <v>15264359805.57265</v>
+        <v>14908279058.42171</v>
       </c>
     </row>
     <row r="155" spans="1:10">
@@ -5394,13 +5394,13 @@
         <v>16</v>
       </c>
       <c r="H155">
-        <v>15291893158.8806</v>
+        <v>15290646434.90685</v>
       </c>
       <c r="I155">
-        <v>23.86960169517343</v>
+        <v>333.1998288522125</v>
       </c>
       <c r="J155">
-        <v>15264113701.9573</v>
+        <v>14906605478.93839</v>
       </c>
     </row>
     <row r="156" spans="1:10">
@@ -5426,13 +5426,13 @@
         <v>17</v>
       </c>
       <c r="H156">
-        <v>15291666255.03229</v>
+        <v>15290337357.97599</v>
       </c>
       <c r="I156">
-        <v>23.84461676080356</v>
+        <v>332.5551969767691</v>
       </c>
       <c r="J156">
-        <v>15263902765.453</v>
+        <v>14907010606.14262</v>
       </c>
     </row>
     <row r="157" spans="1:10">
@@ -5458,13 +5458,13 @@
         <v>18</v>
       </c>
       <c r="H157">
-        <v>15291615479.89652</v>
+        <v>15290266855.62614</v>
       </c>
       <c r="I157">
-        <v>23.76398214001628</v>
+        <v>330.4240721488735</v>
       </c>
       <c r="J157">
-        <v>15263932968.45062</v>
+        <v>14909306066.37149</v>
       </c>
     </row>
     <row r="158" spans="1:10">
@@ -5490,13 +5490,13 @@
         <v>19</v>
       </c>
       <c r="H158">
-        <v>15291677523.23417</v>
+        <v>15290342605.2949</v>
       </c>
       <c r="I158">
-        <v>24.01597539409756</v>
+        <v>332.9994023761273</v>
       </c>
       <c r="J158">
-        <v>15263693446.15138</v>
+        <v>14906464115.88803</v>
       </c>
     </row>
     <row r="159" spans="1:10">
@@ -5522,13 +5522,13 @@
         <v>20</v>
       </c>
       <c r="H159">
-        <v>15291995874.36903</v>
+        <v>15290774012.84996</v>
       </c>
       <c r="I159">
-        <v>24.41367285126583</v>
+        <v>334.7719959555027</v>
       </c>
       <c r="J159">
-        <v>15263578701.33166</v>
+        <v>14904828688.07253</v>
       </c>
     </row>
     <row r="160" spans="1:10">
@@ -5554,13 +5554,13 @@
         <v>21</v>
       </c>
       <c r="H160">
-        <v>15292118157.63056</v>
+        <v>15290941153.21388</v>
       </c>
       <c r="I160">
-        <v>25.18432046828665</v>
+        <v>335.2656000182092</v>
       </c>
       <c r="J160">
-        <v>15262869427.4436</v>
+        <v>14904440893.42135</v>
       </c>
     </row>
     <row r="161" spans="1:10">
@@ -5586,13 +5586,13 @@
         <v>22</v>
       </c>
       <c r="H161">
-        <v>15292117576.09421</v>
+        <v>15290934870.8301</v>
       </c>
       <c r="I161">
-        <v>29.82984208280117</v>
+        <v>336.9025321004047</v>
       </c>
       <c r="J161">
-        <v>15257680196.29526</v>
+        <v>14902549682.61704</v>
       </c>
     </row>
   </sheetData>

</xml_diff>